<commit_message>
write new file instead of updating
</commit_message>
<xml_diff>
--- a/masanduku/samplefile.xlsx
+++ b/masanduku/samplefile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sample" sheetId="1" relationships:id="rId2" state="visible"/>
+    <sheet name="sample" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -604,20 +604,14 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -626,74 +620,74 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <sheetPr>
-    <pageSetUpPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="L1" activeCellId="0" pane="topLeft" sqref="L:L"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L:L"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="11" min="1" style="1" width="11.52"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.52"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row ht="12.8" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="12.8" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>882966</v>
       </c>
@@ -762,11 +756,8 @@
       <c r="K2" s="2" t="n">
         <v>25708</v>
       </c>
-      <c r="L2" t="str">
-        <v>Aaron Mcphail</v>
-      </c>
-    </row>
-    <row ht="12.8" r="3">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>189028</v>
       </c>
@@ -800,11 +791,8 @@
       <c r="K3" s="2" t="n">
         <v>21672</v>
       </c>
-      <c r="L3" t="str">
-        <v>Basil Mccrimmon</v>
-      </c>
-    </row>
-    <row ht="12.8" r="4">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>479122</v>
       </c>
@@ -838,11 +826,8 @@
       <c r="K4" s="2" t="n">
         <v>32050</v>
       </c>
-      <c r="L4" t="str">
-        <v>Bryce Glen</v>
-      </c>
-    </row>
-    <row ht="12.8" r="5">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>484002</v>
       </c>
@@ -876,11 +861,8 @@
       <c r="K5" s="2" t="n">
         <v>26151</v>
       </c>
-      <c r="L5" t="str">
-        <v>Chadwick Karim</v>
-      </c>
-    </row>
-    <row ht="12.8" r="6">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>677207</v>
       </c>
@@ -914,11 +896,8 @@
       <c r="K6" s="2" t="n">
         <v>26044</v>
       </c>
-      <c r="L6" t="str">
-        <v>Clyde Rossignol</v>
-      </c>
-    </row>
-    <row ht="12.8" r="7">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>751833</v>
       </c>
@@ -952,11 +931,8 @@
       <c r="K7" s="2" t="n">
         <v>25042</v>
       </c>
-      <c r="L7" t="str">
-        <v>Dennis Salzman</v>
-      </c>
-    </row>
-    <row ht="12.8" r="8">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>954117</v>
       </c>
@@ -990,11 +966,8 @@
       <c r="K8" s="2" t="n">
         <v>22799</v>
       </c>
-      <c r="L8" t="str">
-        <v>Dominic Reich</v>
-      </c>
-    </row>
-    <row ht="12.8" r="9">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>791004</v>
       </c>
@@ -1028,11 +1001,8 @@
       <c r="K9" s="2" t="n">
         <v>27984</v>
       </c>
-      <c r="L9" t="str">
-        <v>Dwayne Rolfe</v>
-      </c>
-    </row>
-    <row ht="12.8" r="10">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>115794</v>
       </c>
@@ -1066,11 +1036,8 @@
       <c r="K10" s="2" t="n">
         <v>25426</v>
       </c>
-      <c r="L10" t="str">
-        <v>Efren Ealey</v>
-      </c>
-    </row>
-    <row ht="12.8" r="11">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>798499</v>
       </c>
@@ -1104,11 +1071,8 @@
       <c r="K11" s="2" t="n">
         <v>22531</v>
       </c>
-      <c r="L11" t="str">
-        <v>Emil Wadkins</v>
-      </c>
-    </row>
-    <row ht="12.8" r="12">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>936027</v>
       </c>
@@ -1142,11 +1106,8 @@
       <c r="K12" s="2" t="n">
         <v>30477</v>
       </c>
-      <c r="L12" t="str">
-        <v>Isiah Kieffer</v>
-      </c>
-    </row>
-    <row ht="12.8" r="13">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>868441</v>
       </c>
@@ -1180,11 +1141,8 @@
       <c r="K13" s="2" t="n">
         <v>35090</v>
       </c>
-      <c r="L13" t="str">
-        <v>Jay Gebhard</v>
-      </c>
-    </row>
-    <row ht="12.8" r="14">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>425094</v>
       </c>
@@ -1218,11 +1176,8 @@
       <c r="K14" s="2" t="n">
         <v>22516</v>
       </c>
-      <c r="L14" t="str">
-        <v>Joe Mcgeorge</v>
-      </c>
-    </row>
-    <row ht="12.8" r="15">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>749006</v>
       </c>
@@ -1256,11 +1211,8 @@
       <c r="K15" s="2" t="n">
         <v>27559</v>
       </c>
-      <c r="L15" t="str">
-        <v>Lucien Goodwyn</v>
-      </c>
-    </row>
-    <row ht="12.8" r="16">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>962328</v>
       </c>
@@ -1294,11 +1246,8 @@
       <c r="K16" s="2" t="n">
         <v>33595</v>
       </c>
-      <c r="L16" t="str">
-        <v>Lucio Kay</v>
-      </c>
-    </row>
-    <row ht="12.8" r="17">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>489407</v>
       </c>
@@ -1332,11 +1281,8 @@
       <c r="K17" s="2" t="n">
         <v>25570</v>
       </c>
-      <c r="L17" t="str">
-        <v>Marlin Lo</v>
-      </c>
-    </row>
-    <row ht="12.8" r="18">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>907031</v>
       </c>
@@ -1370,11 +1316,8 @@
       <c r="K18" s="2" t="n">
         <v>25711</v>
       </c>
-      <c r="L18" t="str">
-        <v>Merle Lew</v>
-      </c>
-    </row>
-    <row ht="12.8" r="19">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>602022</v>
       </c>
@@ -1408,11 +1351,8 @@
       <c r="K19" s="2" t="n">
         <v>30525</v>
       </c>
-      <c r="L19" t="str">
-        <v>Normand Lindholm</v>
-      </c>
-    </row>
-    <row ht="12.8" r="20">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>395683</v>
       </c>
@@ -1446,11 +1386,8 @@
       <c r="K20" s="2" t="n">
         <v>27492</v>
       </c>
-      <c r="L20" t="str">
-        <v>Porfirio Still</v>
-      </c>
-    </row>
-    <row ht="12.8" r="21">
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>989907</v>
       </c>
@@ -1484,11 +1421,8 @@
       <c r="K21" s="2" t="n">
         <v>31383</v>
       </c>
-      <c r="L21" t="str">
-        <v>Reuben Mitchum</v>
-      </c>
-    </row>
-    <row ht="12.8" r="22">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>559395</v>
       </c>
@@ -1522,11 +1456,8 @@
       <c r="K22" s="2" t="n">
         <v>26765</v>
       </c>
-      <c r="L22" t="str">
-        <v>Rocky River</v>
-      </c>
-    </row>
-    <row ht="12.8" r="23">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>183341</v>
       </c>
@@ -1560,11 +1491,8 @@
       <c r="K23" s="2" t="n">
         <v>34243</v>
       </c>
-      <c r="L23" t="str">
-        <v>Sebastian Etzel</v>
-      </c>
-    </row>
-    <row ht="12.8" r="24">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>925382</v>
       </c>
@@ -1598,11 +1526,8 @@
       <c r="K24" s="2" t="n">
         <v>23270</v>
       </c>
-      <c r="L24" t="str">
-        <v>Vance Corpus</v>
-      </c>
-    </row>
-    <row ht="12.8" r="25">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>913180</v>
       </c>
@@ -1636,11 +1561,8 @@
       <c r="K25" s="2" t="n">
         <v>24313</v>
       </c>
-      <c r="L25" t="str">
-        <v>Wilbur Geren</v>
-      </c>
-    </row>
-    <row ht="12.8" r="26">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>919133</v>
       </c>
@@ -1674,15 +1596,12 @@
       <c r="K26" s="2" t="n">
         <v>27993</v>
       </c>
-      <c r="L26" t="str">
-        <v>Wiley Baltimore</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions gridLinesSet="true"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup cellComments="none" copies="1" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
using goroutines to sort fathersnames from excel
</commit_message>
<xml_diff>
--- a/masanduku/samplefile.xlsx
+++ b/masanduku/samplefile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="183">
   <si>
     <t xml:space="preserve">EmpID</t>
   </si>
@@ -644,11 +644,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -674,926 +670,1064 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L:L"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="31:31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="0" t="n">
         <v>882966</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>25708</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="0" t="n">
         <v>189028</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>21672</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="0" t="n">
         <v>479122</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>32050</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="0" t="n">
         <v>484002</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>26151</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="0" t="n">
         <v>677207</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="1" t="n">
         <v>26044</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="0" t="n">
         <v>751833</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="1" t="n">
         <v>25042</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="0" t="n">
         <v>954117</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="1" t="n">
         <v>22799</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="0" t="n">
         <v>791004</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="K9" s="1" t="n">
         <v>27984</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="0" t="n">
         <v>115794</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="1" t="n">
         <v>25426</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="0" t="n">
         <v>798499</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="1" t="n">
         <v>22531</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="0" t="n">
         <v>936027</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="K12" s="2" t="n">
+      <c r="K12" s="1" t="n">
         <v>30477</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="0" t="n">
         <v>868441</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="K13" s="1" t="n">
         <v>35090</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="0" t="n">
         <v>425094</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" s="1" t="n">
         <v>22516</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="0" t="n">
         <v>749006</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="2" t="n">
+      <c r="K15" s="1" t="n">
         <v>27559</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="0" t="n">
         <v>962328</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="2" t="n">
+      <c r="K16" s="1" t="n">
         <v>33595</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="0" t="n">
         <v>489407</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="2" t="n">
+      <c r="K17" s="1" t="n">
         <v>25570</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="0" t="n">
         <v>907031</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="K18" s="2" t="n">
+      <c r="K18" s="1" t="n">
         <v>25711</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="0" t="n">
         <v>602022</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="K19" s="2" t="n">
+      <c r="K19" s="1" t="n">
         <v>30525</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="0" t="n">
         <v>395683</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="K20" s="2" t="n">
+      <c r="K20" s="1" t="n">
         <v>27492</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="0" t="n">
         <v>989907</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="K21" s="2" t="n">
+      <c r="K21" s="1" t="n">
         <v>31383</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="0" t="n">
         <v>559395</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="K22" s="2" t="n">
+      <c r="K22" s="1" t="n">
         <v>26765</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="0" t="n">
         <v>183341</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="K23" s="2" t="n">
+      <c r="K23" s="1" t="n">
         <v>34243</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="0" t="n">
         <v>925382</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="K24" s="2" t="n">
+      <c r="K24" s="1" t="n">
         <v>23270</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="0" t="n">
         <v>913180</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="K25" s="2" t="n">
+      <c r="K25" s="1" t="n">
         <v>24313</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="0" t="n">
         <v>919133</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="K26" s="2" t="n">
+      <c r="K26" s="1" t="n">
+        <v>27993</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>919133</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>27993</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>925382</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>23270</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>913180</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>24313</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>919133</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="K30" s="1" t="n">
         <v>27993</v>
       </c>
     </row>

</xml_diff>